<commit_message>
Optimized Code In Python Main Program
</commit_message>
<xml_diff>
--- a/Excel/Bulanan/Excel/List Tugas Bulanan Ke-3 (4 Oktober 2021 - 8 November 2021).xlsx
+++ b/Excel/Bulanan/Excel/List Tugas Bulanan Ke-3 (4 Oktober 2021 - 8 November 2021).xlsx
@@ -551,7 +551,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R10" sqref="Q10:R13"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -781,7 +781,11 @@
           <t>Muhammad Athala Romero</t>
         </is>
       </c>
-      <c r="C19" s="17" t="inlineStr"/>
+      <c r="C19" s="18" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="20" ht="15.6" customHeight="1">
       <c r="A20" s="11" t="n">

</xml_diff>